<commit_message>
agrego cambios de pedidos
</commit_message>
<xml_diff>
--- a/Tarifario.xlsx
+++ b/Tarifario.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="25726"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CCE558D7-6E23-418E-AAC7-AD52CFA072F0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3A7DA6F3-0BF9-417F-A0E2-2C25B99169B5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -28,23 +28,11 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="26">
   <si>
     <t>Precio por unidad (bulto)</t>
   </si>
   <si>
-    <t>Local</t>
-  </si>
-  <si>
-    <t>Provincial</t>
-  </si>
-  <si>
-    <t>Regional</t>
-  </si>
-  <si>
-    <t>Nacional</t>
-  </si>
-  <si>
     <t>Sobres hasta 500g</t>
   </si>
   <si>
@@ -103,6 +91,21 @@
   </si>
   <si>
     <t>Region Norte (sede Resistencia) -&gt; Chaco, Misiones, Corrientes, Santiago del estero, Formosa, Jujuy, Salta, Tucuman y Catamarca</t>
+  </si>
+  <si>
+    <t>Region Metropolitana (sede CABA) -&gt; Buenos Aires</t>
+  </si>
+  <si>
+    <t>Local (misma localidad)</t>
+  </si>
+  <si>
+    <t>Provincial (misma provincia)</t>
+  </si>
+  <si>
+    <t>Regional (misma región)</t>
+  </si>
+  <si>
+    <t>Nacional (inter-regional)</t>
   </si>
 </sst>
 </file>
@@ -532,16 +535,20 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="B1:J20"/>
+  <dimension ref="B1:J21"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="G20" sqref="G20"/>
+      <selection activeCell="C18" sqref="C18:C21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="2" max="2" width="34.42578125" customWidth="1"/>
-    <col min="3" max="7" width="19.5703125" customWidth="1"/>
+    <col min="3" max="3" width="21.85546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="26.42578125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="22.85546875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="23.140625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="19.5703125" customWidth="1"/>
     <col min="9" max="9" width="16.85546875" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="30.85546875" customWidth="1"/>
   </cols>
@@ -556,36 +563,36 @@
       <c r="E2" s="10"/>
       <c r="F2" s="10"/>
       <c r="I2" s="6" t="s">
-        <v>14</v>
+        <v>10</v>
       </c>
       <c r="J2" s="6" t="s">
-        <v>15</v>
+        <v>11</v>
       </c>
     </row>
     <row r="3" spans="2:10" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B3" s="1"/>
       <c r="C3" s="2" t="s">
-        <v>1</v>
+        <v>22</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>2</v>
+        <v>23</v>
       </c>
       <c r="E3" s="2" t="s">
-        <v>3</v>
+        <v>24</v>
       </c>
       <c r="F3" s="2" t="s">
-        <v>4</v>
+        <v>25</v>
       </c>
       <c r="I3" s="7" t="s">
-        <v>16</v>
+        <v>12</v>
       </c>
       <c r="J3" s="8" t="s">
-        <v>19</v>
+        <v>15</v>
       </c>
     </row>
     <row r="4" spans="2:10" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B4" s="3" t="s">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="C4" s="4">
         <v>350</v>
@@ -601,15 +608,15 @@
       </c>
       <c r="G4" s="5"/>
       <c r="I4" s="9" t="s">
+        <v>13</v>
+      </c>
+      <c r="J4" s="8" t="s">
         <v>17</v>
-      </c>
-      <c r="J4" s="8" t="s">
-        <v>21</v>
       </c>
     </row>
     <row r="5" spans="2:10" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B5" s="3" t="s">
-        <v>6</v>
+        <v>2</v>
       </c>
       <c r="C5" s="4">
         <f>+C4*10</f>
@@ -629,15 +636,15 @@
       </c>
       <c r="G5" s="5"/>
       <c r="I5" s="9" t="s">
-        <v>18</v>
+        <v>14</v>
       </c>
       <c r="J5" s="8" t="s">
-        <v>20</v>
+        <v>16</v>
       </c>
     </row>
     <row r="6" spans="2:10" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B6" s="3" t="s">
-        <v>7</v>
+        <v>3</v>
       </c>
       <c r="C6" s="4">
         <f>+C4*12</f>
@@ -659,7 +666,7 @@
     </row>
     <row r="7" spans="2:10" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B7" s="3" t="s">
-        <v>8</v>
+        <v>4</v>
       </c>
       <c r="C7" s="4">
         <f>+C4*15</f>
@@ -708,24 +715,24 @@
     <row r="11" spans="2:10" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B11" s="4"/>
       <c r="C11" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="D11" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="E11" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="F11" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="G11" s="4" t="s">
         <v>9</v>
-      </c>
-      <c r="D11" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="E11" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="F11" s="4" t="s">
-        <v>12</v>
-      </c>
-      <c r="G11" s="4" t="s">
-        <v>13</v>
       </c>
     </row>
     <row r="12" spans="2:10" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B12" s="3" t="s">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="C12" s="4">
         <v>1620</v>
@@ -745,7 +752,7 @@
     </row>
     <row r="13" spans="2:10" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B13" s="3" t="s">
-        <v>6</v>
+        <v>2</v>
       </c>
       <c r="C13" s="4">
         <f>+C12*10</f>
@@ -770,7 +777,7 @@
     </row>
     <row r="14" spans="2:10" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B14" s="3" t="s">
-        <v>7</v>
+        <v>3</v>
       </c>
       <c r="C14" s="4">
         <f>+C12*12</f>
@@ -795,7 +802,7 @@
     </row>
     <row r="15" spans="2:10" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B15" s="3" t="s">
-        <v>8</v>
+        <v>4</v>
       </c>
       <c r="C15" s="4">
         <f>+C12*15</f>
@@ -820,17 +827,22 @@
     </row>
     <row r="18" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B18" t="s">
-        <v>22</v>
+        <v>18</v>
       </c>
     </row>
     <row r="19" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B19" t="s">
-        <v>23</v>
+        <v>19</v>
       </c>
     </row>
     <row r="20" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B20" t="s">
-        <v>24</v>
+        <v>20</v>
+      </c>
+    </row>
+    <row r="21" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B21" t="s">
+        <v>21</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
agregamos localidades por provincia
</commit_message>
<xml_diff>
--- a/Tarifario.xlsx
+++ b/Tarifario.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="25726"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3A7DA6F3-0BF9-417F-A0E2-2C25B99169B5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{953159A5-F3CA-4005-B9AE-46A9C9D83D92}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -538,7 +538,7 @@
   <dimension ref="B1:J21"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="C18" sqref="C18:C21"/>
+      <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -856,6 +856,27 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <Unidad xmlns="d1a0e966-e597-44cd-ac53-f1d0c001247b" xsi:nil="true"/>
+    <Comentarios xmlns="d1a0e966-e597-44cd-ac53-f1d0c001247b" xsi:nil="true"/>
+    <Fecha_x0020_Publicacion xmlns="d1a0e966-e597-44cd-ac53-f1d0c001247b">2022-11-03T03:00:00+00:00</Fecha_x0020_Publicacion>
+    <Nro xmlns="d1a0e966-e597-44cd-ac53-f1d0c001247b">5</Nro>
+    <Vence xmlns="d1a0e966-e597-44cd-ac53-f1d0c001247b" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Documento" ma:contentTypeID="0x01010011E9A24E4DE0C042AA03CB85C89E33F3" ma:contentTypeVersion="9" ma:contentTypeDescription="Crear nuevo documento." ma:contentTypeScope="" ma:versionID="ae5ee57c3f0a87dc4959a64fdfc56c1b">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="d1a0e966-e597-44cd-ac53-f1d0c001247b" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="e479666f1da18a33536c4f94ef1b5e15" ns2:_="">
     <xsd:import namespace="d1a0e966-e597-44cd-ac53-f1d0c001247b"/>
@@ -1031,28 +1052,25 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <Unidad xmlns="d1a0e966-e597-44cd-ac53-f1d0c001247b" xsi:nil="true"/>
-    <Comentarios xmlns="d1a0e966-e597-44cd-ac53-f1d0c001247b" xsi:nil="true"/>
-    <Fecha_x0020_Publicacion xmlns="d1a0e966-e597-44cd-ac53-f1d0c001247b">2022-11-03T03:00:00+00:00</Fecha_x0020_Publicacion>
-    <Nro xmlns="d1a0e966-e597-44cd-ac53-f1d0c001247b">5</Nro>
-    <Vence xmlns="d1a0e966-e597-44cd-ac53-f1d0c001247b" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{F5C48A8E-4566-4070-ACB8-09EB4F97F4C5}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{817C645C-91AB-4860-A962-09484E532BD2}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="d1a0e966-e597-44cd-ac53-f1d0c001247b"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{B2671DD7-05C2-4CE4-AA81-3DBE99193727}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -1068,22 +1086,4 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{817C645C-91AB-4860-A962-09484E532BD2}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="d1a0e966-e597-44cd-ac53-f1d0c001247b"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{F5C48A8E-4566-4070-ACB8-09EB4F97F4C5}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>